<commit_message>
delete IDC from family tree site
</commit_message>
<xml_diff>
--- a/hed/addenda/idc1.xlsx
+++ b/hed/addenda/idc1.xlsx
@@ -262,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -270,11 +270,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -294,18 +303,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,61 +614,61 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D16"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="24.75" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25">
+    <row r="2" spans="1:4" ht="24.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:4" ht="24.75" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25">
+    <row r="4" spans="1:4" ht="24.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -672,7 +682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25">
+    <row r="5" spans="1:4" ht="24.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -686,7 +696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25">
+    <row r="6" spans="1:4" ht="24.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -700,7 +710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25">
+    <row r="7" spans="1:4" ht="24.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -714,7 +724,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25">
+    <row r="8" spans="1:4" ht="24.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -728,7 +738,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -742,7 +752,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.25">
+    <row r="10" spans="1:4" ht="24.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
@@ -756,7 +766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.25">
+    <row r="11" spans="1:4" ht="24.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
@@ -770,7 +780,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25">
+    <row r="12" spans="1:4" ht="24.75" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -784,7 +794,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25">
+    <row r="13" spans="1:4" ht="24.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
@@ -794,17 +804,17 @@
       <c r="C13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" ht="16.5">
+    <row r="14" spans="1:4" ht="24.75" customHeight="1">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4" ht="24.75" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
@@ -812,7 +822,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="16.5">
+    <row r="16" spans="1:4" ht="24.75" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>51</v>
       </c>
@@ -826,9 +836,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <webPublishItems count="2">
+  <webPublishItems count="3">
+    <webPublishItem id="25212" divId="idc1_25212" sourceType="sheet" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addenda\idc1.htm" title="Ideographic Description Characters (IDC)"/>
     <webPublishItem id="28383" divId="idc1_28383" sourceType="range" sourceRef="A1:D16" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addendum\idc1.htm"/>
-    <webPublishItem id="20249" divId="Book1_20249" sourceType="range" sourceRef="A1:D16" destinationFile="C:\Users\Gene\Documents\GitHub\chinfamilytree.github.io\hed\addendum\idc1.htm" title="Ideographic Description Characters (IDC)"/>
+    <webPublishItem id="20249" divId="Book1_20249" sourceType="range" sourceRef="A1:D16" destinationFile="C:\Users\Gene\Documents\idc1.htm" title="Ideographic Description Characters (IDC)"/>
   </webPublishItems>
 </worksheet>
 </file>

</xml_diff>